<commit_message>
📦 build(root): update gitignore, vscode settings, docs, and dependencies
- add repomix output to gitignore
- add vscode settings for python analysis
- update documentation for project structure and dependencies
- update readme for project features and installation
- add technical task pdf
- add input excel files
- update separate into files script
- update unittests script
- update utils script
- update xlsx to kml script
</commit_message>
<xml_diff>
--- a/input/Москва_fixed.xlsx
+++ b/input/Москва_fixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!WORK\!Programming\Excel_to_KML\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3C7B01-EF38-48B5-8A68-FA85E6ABCA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E38FB4C-A98A-470F-BF4E-26108F6B5C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E9A61020-BC2E-4C1B-989B-00EFA3FE8BDA}"/>
   </bookViews>
@@ -4161,7 +4161,7 @@
 8: 14899.14м, -9734.00м</t>
   </si>
   <si>
-    <t>  Московская СК г. Москва, Южный а.о., пр-кт Андропова 1: 2405.0м., 1100.0м.2: 2648.7м., 11424.56м.3: 2618.04м., 11442.93м.4: 2369.1м., 1108.16м.</t>
+    <t>  Московская СК г. Москва, Южный а.о., пр-кт Андропова 1: 2405.0м., 11000.0м.2: 2648.7м., 11424.56м.3: 2618.04м., 11442.93м.4: 2369.1м., 11008.16м.</t>
   </si>
 </sst>
 </file>
@@ -5135,7 +5135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D76DD66-070A-4A88-942B-495BBA04E573}">
   <dimension ref="A1:T248"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A168" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C168" workbookViewId="0">
       <selection activeCell="H168" sqref="H168"/>
     </sheetView>
   </sheetViews>

</xml_diff>